<commit_message>
Integrate new data source for fuels/ETRbF
</commit_message>
<xml_diff>
--- a/InputData/fuels/ETRbF/Export Tax Rate by Fuel.xlsx
+++ b/InputData/fuels/ETRbF/Export Tax Rate by Fuel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\fuels\ETRbF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\fuels\ETRbF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46292268-5F85-4F58-AA12-4C637BB2BFCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="9795"/>
+    <workbookView xWindow="6630" yWindow="-15555" windowWidth="18945" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,26 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>Patrick Watson</t>
-  </si>
-  <si>
-    <t>The U.S. Has Never Had a Tax on Exports</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>According to Encyclopedia Britannica:</t>
   </si>
   <si>
-    <t>https://www.forbes.com/sites/patrickwwatson/2017/02/13/the-us-has-never-had-a-tax-on-exports/</t>
-  </si>
-  <si>
     <t>Export duties are no longer used to a great extent, except to tax certain mineral, petroleum, and agricultural</t>
   </si>
   <si>
@@ -124,12 +116,33 @@
   </si>
   <si>
     <t>Export Tax Rate (dimensionless)</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>VAT rules and rates</t>
+  </si>
+  <si>
+    <t>https://europa.eu/youreurope/business/taxation/vat/vat-rules-rates/index_en.htm</t>
+  </si>
+  <si>
+    <t>Goods exported from the EU to non-EU countries are VAT-exempt.</t>
+  </si>
+  <si>
+    <t>https://trade.ec.europa.eu/access-to-markets/en/content/</t>
+  </si>
+  <si>
+    <t>Access2Markets (official European Commission website)</t>
+  </si>
+  <si>
+    <t>Site has detailed information on tariffs, taxes, and duties by product. (VPN required for acess outside of EU.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,18 +195,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,10 +490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -486,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -494,73 +512,108 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3">
-        <v>2017</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>8</v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="A11" r:id="rId2" location="ref592273" display="https://www.britannica.com/topic/tariff - ref592273"/>
+    <hyperlink ref="A16" r:id="rId1" location="ref592273" display="https://www.britannica.com/topic/tariff - ref592273" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{5E171150-EEBC-40DF-8F33-88C5D9FD2472}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{60C9E263-8895-4824-A767-ECFE6CDDECFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -570,134 +623,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1"/>
-      <c r="B1" s="4" t="s">
-        <v>32</v>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -705,7 +758,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -713,7 +766,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -721,7 +774,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -729,7 +782,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -737,7 +790,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -745,5 +798,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>